<commit_message>
add 1.3.0 dev kit docu
</commit_message>
<xml_diff>
--- a/docs/development-kit/html5-documentation-data-service-development-kit/ProductionSummary.xlsx
+++ b/docs/development-kit/html5-documentation-data-service-development-kit/ProductionSummary.xlsx
@@ -8,7 +8,7 @@
     <t xml:space="preserve">Produktionszeitpunkt</t>
   </si>
   <si>
-    <t xml:space="preserve">02.08.2021 08:23:28</t>
+    <t xml:space="preserve">08.09.2021 11:58:39</t>
   </si>
   <si>
     <t xml:space="preserve">Systeminformation</t>
@@ -77,13 +77,13 @@
     <t xml:space="preserve">Knoten-ID</t>
   </si>
   <si>
-    <t xml:space="preserve">147624130955</t>
+    <t xml:space="preserve">148678453899</t>
   </si>
   <si>
     <t xml:space="preserve">Titel</t>
   </si>
   <si>
-    <t xml:space="preserve">Data Service Development Kit for Industrial Edge</t>
+    <t xml:space="preserve">Data Service Development Kit for Industrial Edge V1.3</t>
   </si>
   <si>
     <t xml:space="preserve">Dateiname</t>
@@ -107,7 +107,7 @@
     <t xml:space="preserve">Ausgabestand</t>
   </si>
   <si>
-    <t xml:space="preserve">07/2021</t>
+    <t xml:space="preserve">09/2021</t>
   </si>
   <si>
     <t xml:space="preserve">Copyright-Jahreszahlen</t>
@@ -122,7 +122,7 @@
     <t xml:space="preserve">Dokument-Identifikationsnummer</t>
   </si>
   <si>
-    <t xml:space="preserve">A5E50909565-AB</t>
+    <t xml:space="preserve">A5E50909565-AC</t>
   </si>
   <si>
     <t xml:space="preserve">Innentitel-Infofeld</t>
@@ -140,7 +140,7 @@
     <t xml:space="preserve">PDF verlinken</t>
   </si>
   <si>
-    <t xml:space="preserve">UEsDBBQAAAAIAO5CAlPi/LD+YAAAAGsAAAALAAAAc3lzRGF0YS54bWx7v3u/jX1Fbo5CWWpRcWZ+nq2SoZ6BkkJqXnJ+SmZeuq1SaUmaroWSQnFJYl5KYk5+XqqtUmVqsZK9nU1KYkkisjZDoE49Y3NDSyU7m4Ki/ILUopLM1GIFfTsbfZBSOwBQSwECFAAUAAAACADuQgJT4vyw/mAAAABrAAAACwAAAAAAAAAAAAAAAAAAAAAAc3lzRGF0YS54bWxQSwUGAAAAAAEAAQA5AAAAiQAAAAAA</t>
+    <t xml:space="preserve">UEsDBBQAAAAIAFNfKFPi/LD+YAAAAGsAAAALAAAAc3lzRGF0YS54bWx7v3u/jX1Fbo5CWWpRcWZ+nq2SoZ6BkkJqXnJ+SmZeuq1SaUmaroWSQnFJYl5KYk5+XqqtUmVqsZK9nU1KYkkisjZDoE49Y3NDSyU7m4Ki/ILUopLM1GIFfTsbfZBSOwBQSwECFAAUAAAACABTXyhT4vyw/mAAAABrAAAACwAAAAAAAAAAAAAAAAAAAAAAc3lzRGF0YS54bWxQSwUGAAAAAAEAAQA5AAAAiQAAAAAA</t>
   </si>
 </sst>
 </file>
@@ -332,7 +332,7 @@
         <v>24</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>147624130955</v>
+        <v>148678453899</v>
       </c>
     </row>
     <row r="20">

</xml_diff>

<commit_message>
add 1.6.0 devkit docu
</commit_message>
<xml_diff>
--- a/docs/development-kit/html5-documentation-data-service-development-kit/ProductionSummary.xlsx
+++ b/docs/development-kit/html5-documentation-data-service-development-kit/ProductionSummary.xlsx
@@ -8,13 +8,13 @@
     <t xml:space="preserve">Produktionszeitpunkt</t>
   </si>
   <si>
-    <t xml:space="preserve">21.11.2022 13:03:44</t>
+    <t xml:space="preserve">04.04.2023 09:09:41</t>
   </si>
   <si>
     <t xml:space="preserve">Systeminformation</t>
   </si>
   <si>
-    <t xml:space="preserve">R38a-18</t>
+    <t xml:space="preserve">R38c-03</t>
   </si>
   <si>
     <t xml:space="preserve">Produktion</t>
@@ -26,7 +26,7 @@
     <t xml:space="preserve">Produktionssprache</t>
   </si>
   <si>
-    <t xml:space="preserve">de-DE, en-US, zh-CHS, es-ES</t>
+    <t xml:space="preserve">de-DE, en-US, fr-FR, it-IT, es-ES, zh-CHS</t>
   </si>
   <si>
     <t xml:space="preserve">Warnhinweis-Layout</t>
@@ -50,6 +50,9 @@
     <t xml:space="preserve">IDs an Topic-Titel anfügen</t>
   </si>
   <si>
+    <t xml:space="preserve">Ja</t>
+  </si>
+  <si>
     <t xml:space="preserve">Temporäre Dateien löschen</t>
   </si>
   <si>
@@ -74,19 +77,19 @@
     <t xml:space="preserve">Knoten-ID</t>
   </si>
   <si>
-    <t xml:space="preserve">162961708683</t>
+    <t xml:space="preserve">167072438667</t>
   </si>
   <si>
     <t xml:space="preserve">Titel</t>
   </si>
   <si>
-    <t xml:space="preserve">Data Service Development Kit for Industrial Edge V1.5</t>
+    <t xml:space="preserve">Data Service Development Kit for Industrial Edge V1.6</t>
   </si>
   <si>
     <t xml:space="preserve">Dateiname</t>
   </si>
   <si>
-    <t xml:space="preserve">EdgeApp_DevelopmentKitdeDE</t>
+    <t xml:space="preserve">EdgeApp_DevelopmentKit_deDE</t>
   </si>
   <si>
     <t xml:space="preserve">System</t>
@@ -104,13 +107,13 @@
     <t xml:space="preserve">Ausgabestand</t>
   </si>
   <si>
-    <t xml:space="preserve">11/2022; V1.5</t>
+    <t xml:space="preserve">03/2023; V1.6</t>
   </si>
   <si>
     <t xml:space="preserve">Copyright-Jahreszahlen</t>
   </si>
   <si>
-    <t xml:space="preserve">2021 - 2022</t>
+    <t xml:space="preserve">2021 - 2023</t>
   </si>
   <si>
     <t xml:space="preserve">Dokument-Bestellnummer</t>
@@ -119,7 +122,7 @@
     <t xml:space="preserve">Dokument-Identifikationsnummer</t>
   </si>
   <si>
-    <t xml:space="preserve">A5E50909565-AD</t>
+    <t xml:space="preserve">A5E50909565-AE</t>
   </si>
   <si>
     <t xml:space="preserve">Innentitel-Infofeld</t>
@@ -137,7 +140,7 @@
     <t xml:space="preserve">PDF verlinken</t>
   </si>
   <si>
-    <t xml:space="preserve">UEsDBBQAAAAIAHZodVXi/LD+YAAAAGsAAAALAAAAc3lzRGF0YS54bWx7v3u/jX1Fbo5CWWpRcWZ+nq2SoZ6BkkJqXnJ+SmZeuq1SaUmaroWSQnFJYl5KYk5+XqqtUmVqsZK9nU1KYkkisjZDoE49Y3NDSyU7m4Ki/ILUopLM1GIFfTsbfZBSOwBQSwECFAAUAAAACAB2aHVV4vyw/mAAAABrAAAACwAAAAAAAAAAAAAAAAAAAAAAc3lzRGF0YS54bWxQSwUGAAAAAAEAAQA5AAAAiQAAAAAA</t>
+    <t xml:space="preserve">UEsDBBQAAAAIADRJhFbi/LD+YAAAAGsAAAALAAAAc3lzRGF0YS54bWx7v3u/jX1Fbo5CWWpRcWZ+nq2SoZ6BkkJqXnJ+SmZeuq1SaUmaroWSQnFJYl5KYk5+XqqtUmVqsZK9nU1KYkkisjZDoE49Y3NDSyU7m4Ki/ILUopLM1GIFfTsbfZBSOwBQSwECFAAUAAAACAA0SYRW4vyw/mAAAABrAAAACwAAAAAAAAAAAAAAAAAAAAAAc3lzRGF0YS54bWxQSwUGAAAAAAEAAQA5AAAAiQAAAAAA</t>
   </si>
 </sst>
 </file>
@@ -268,28 +271,28 @@
         <v>15</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="0" t="s">
         <v>16</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>12</v>
@@ -297,13 +300,13 @@
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B14" s="0" t="s"/>
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B15" s="0" t="s"/>
       <c r="C15" s="0" t="s"/>
@@ -314,109 +317,109 @@
     </row>
     <row r="17">
       <c r="A17" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B17" s="0" t="s"/>
     </row>
     <row r="18">
       <c r="A18" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B18" s="0" t="s"/>
     </row>
     <row r="19">
       <c r="A19" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>162961708683</v>
+        <v>167072438667</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B26" s="0" t="s"/>
     </row>
     <row r="27">
       <c r="A27" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B28" s="0" t="s"/>
     </row>
     <row r="29">
       <c r="A29" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B30" s="0" t="s"/>
     </row>
     <row r="31">
       <c r="A31" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B31" s="0" t="s">
         <v>12</v>
@@ -431,7 +434,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
release of IIH Essentials 1.8.0
</commit_message>
<xml_diff>
--- a/docs/development-kit/html5-documentation-data-service-development-kit/ProductionSummary.xlsx
+++ b/docs/development-kit/html5-documentation-data-service-development-kit/ProductionSummary.xlsx
@@ -8,13 +8,13 @@
     <t xml:space="preserve">Produktionszeitpunkt</t>
   </si>
   <si>
-    <t xml:space="preserve">06.06.2023 12:10:57</t>
+    <t xml:space="preserve">22.08.2023 14:02:16</t>
   </si>
   <si>
     <t xml:space="preserve">Systeminformation</t>
   </si>
   <si>
-    <t xml:space="preserve">R38c-03</t>
+    <t xml:space="preserve">R39b-04</t>
   </si>
   <si>
     <t xml:space="preserve">Produktion</t>
@@ -38,12 +38,15 @@
     <t xml:space="preserve">Rückgriff auf veraltete Übersetzungen</t>
   </si>
   <si>
+    <t xml:space="preserve">Ja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indexdatei erzeugen</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nein</t>
   </si>
   <si>
-    <t xml:space="preserve">Indexdatei erzeugen</t>
-  </si>
-  <si>
     <t xml:space="preserve">Standard-Dateinamen verwenden (ID als Dokumentname)</t>
   </si>
   <si>
@@ -53,9 +56,6 @@
     <t xml:space="preserve">Temporäre Dateien löschen</t>
   </si>
   <si>
-    <t xml:space="preserve">Ja</t>
-  </si>
-  <si>
     <t xml:space="preserve">Layoutvariante</t>
   </si>
   <si>
@@ -77,13 +77,13 @@
     <t xml:space="preserve">Knoten-ID</t>
   </si>
   <si>
-    <t xml:space="preserve">169422809867</t>
+    <t xml:space="preserve">171973069195</t>
   </si>
   <si>
     <t xml:space="preserve">Titel</t>
   </si>
   <si>
-    <t xml:space="preserve">Data Service Development Kit for Industrial Edge V1.7</t>
+    <t xml:space="preserve">Data Service Development Kit for Industrial Edge V1.8</t>
   </si>
   <si>
     <t xml:space="preserve">Dateiname</t>
@@ -107,13 +107,13 @@
     <t xml:space="preserve">Ausgabestand</t>
   </si>
   <si>
-    <t xml:space="preserve">06/2023; V1.7</t>
+    <t xml:space="preserve">08/2023; V1.8</t>
   </si>
   <si>
     <t xml:space="preserve">Copyright-Jahreszahlen</t>
   </si>
   <si>
-    <t xml:space="preserve">2021 - 2023</t>
+    <t xml:space="preserve">2023</t>
   </si>
   <si>
     <t xml:space="preserve">Dokument-Bestellnummer</t>
@@ -122,7 +122,7 @@
     <t xml:space="preserve">Dokument-Identifikationsnummer</t>
   </si>
   <si>
-    <t xml:space="preserve">A5E50909565-AF</t>
+    <t xml:space="preserve">A5E50909565-AG</t>
   </si>
   <si>
     <t xml:space="preserve">Innentitel-Infofeld</t>
@@ -140,7 +140,7 @@
     <t xml:space="preserve">PDF verlinken</t>
   </si>
   <si>
-    <t xml:space="preserve">UEsDBBQAAAAIAF1hxlbi/LD+YAAAAGsAAAALAAAAc3lzRGF0YS54bWx7v3u/jX1Fbo5CWWpRcWZ+nq2SoZ6BkkJqXnJ+SmZeuq1SaUmaroWSQnFJYl5KYk5+XqqtUmVqsZK9nU1KYkkisjZDoE49Y3NDSyU7m4Ki/ILUopLM1GIFfTsbfZBSOwBQSwECFAAUAAAACABdYcZW4vyw/mAAAABrAAAACwAAAAAAAAAAAAAAAAAAAAAAc3lzRGF0YS54bWxQSwUGAAAAAAEAAQA5AAAAiQAAAAAA</t>
+    <t xml:space="preserve">UEsDBBQAAAAIAEhwFlfi/LD+YAAAAGsAAAALAAAAc3lzRGF0YS54bWx7v3u/jX1Fbo5CWWpRcWZ+nq2SoZ6BkkJqXnJ+SmZeuq1SaUmaroWSQnFJYl5KYk5+XqqtUmVqsZK9nU1KYkkisjZDoE49Y3NDSyU7m4Ki/ILUopLM1GIFfTsbfZBSOwBQSwECFAAUAAAACABIcBZX4vyw/mAAAABrAAAACwAAAAAAAAAAAAAAAAAAAAAAc3lzRGF0YS54bWxQSwUGAAAAAAEAAQA5AAAAiQAAAAAA</t>
   </si>
 </sst>
 </file>
@@ -255,31 +255,31 @@
         <v>13</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="0" t="s">
         <v>14</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12">
@@ -295,7 +295,7 @@
         <v>20</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14">
@@ -332,7 +332,7 @@
         <v>24</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>169422809867</v>
+        <v>171973069195</v>
       </c>
     </row>
     <row r="20">
@@ -422,7 +422,7 @@
         <v>45</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Release 1 8 0 (#16)
* release of IIH Essentials 1.8.0

* 1.8.0 changelog
</commit_message>
<xml_diff>
--- a/docs/development-kit/html5-documentation-data-service-development-kit/ProductionSummary.xlsx
+++ b/docs/development-kit/html5-documentation-data-service-development-kit/ProductionSummary.xlsx
@@ -8,13 +8,13 @@
     <t xml:space="preserve">Produktionszeitpunkt</t>
   </si>
   <si>
-    <t xml:space="preserve">06.06.2023 12:10:57</t>
+    <t xml:space="preserve">22.08.2023 14:02:16</t>
   </si>
   <si>
     <t xml:space="preserve">Systeminformation</t>
   </si>
   <si>
-    <t xml:space="preserve">R38c-03</t>
+    <t xml:space="preserve">R39b-04</t>
   </si>
   <si>
     <t xml:space="preserve">Produktion</t>
@@ -38,12 +38,15 @@
     <t xml:space="preserve">Rückgriff auf veraltete Übersetzungen</t>
   </si>
   <si>
+    <t xml:space="preserve">Ja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indexdatei erzeugen</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nein</t>
   </si>
   <si>
-    <t xml:space="preserve">Indexdatei erzeugen</t>
-  </si>
-  <si>
     <t xml:space="preserve">Standard-Dateinamen verwenden (ID als Dokumentname)</t>
   </si>
   <si>
@@ -53,9 +56,6 @@
     <t xml:space="preserve">Temporäre Dateien löschen</t>
   </si>
   <si>
-    <t xml:space="preserve">Ja</t>
-  </si>
-  <si>
     <t xml:space="preserve">Layoutvariante</t>
   </si>
   <si>
@@ -77,13 +77,13 @@
     <t xml:space="preserve">Knoten-ID</t>
   </si>
   <si>
-    <t xml:space="preserve">169422809867</t>
+    <t xml:space="preserve">171973069195</t>
   </si>
   <si>
     <t xml:space="preserve">Titel</t>
   </si>
   <si>
-    <t xml:space="preserve">Data Service Development Kit for Industrial Edge V1.7</t>
+    <t xml:space="preserve">Data Service Development Kit for Industrial Edge V1.8</t>
   </si>
   <si>
     <t xml:space="preserve">Dateiname</t>
@@ -107,13 +107,13 @@
     <t xml:space="preserve">Ausgabestand</t>
   </si>
   <si>
-    <t xml:space="preserve">06/2023; V1.7</t>
+    <t xml:space="preserve">08/2023; V1.8</t>
   </si>
   <si>
     <t xml:space="preserve">Copyright-Jahreszahlen</t>
   </si>
   <si>
-    <t xml:space="preserve">2021 - 2023</t>
+    <t xml:space="preserve">2023</t>
   </si>
   <si>
     <t xml:space="preserve">Dokument-Bestellnummer</t>
@@ -122,7 +122,7 @@
     <t xml:space="preserve">Dokument-Identifikationsnummer</t>
   </si>
   <si>
-    <t xml:space="preserve">A5E50909565-AF</t>
+    <t xml:space="preserve">A5E50909565-AG</t>
   </si>
   <si>
     <t xml:space="preserve">Innentitel-Infofeld</t>
@@ -140,7 +140,7 @@
     <t xml:space="preserve">PDF verlinken</t>
   </si>
   <si>
-    <t xml:space="preserve">UEsDBBQAAAAIAF1hxlbi/LD+YAAAAGsAAAALAAAAc3lzRGF0YS54bWx7v3u/jX1Fbo5CWWpRcWZ+nq2SoZ6BkkJqXnJ+SmZeuq1SaUmaroWSQnFJYl5KYk5+XqqtUmVqsZK9nU1KYkkisjZDoE49Y3NDSyU7m4Ki/ILUopLM1GIFfTsbfZBSOwBQSwECFAAUAAAACABdYcZW4vyw/mAAAABrAAAACwAAAAAAAAAAAAAAAAAAAAAAc3lzRGF0YS54bWxQSwUGAAAAAAEAAQA5AAAAiQAAAAAA</t>
+    <t xml:space="preserve">UEsDBBQAAAAIAEhwFlfi/LD+YAAAAGsAAAALAAAAc3lzRGF0YS54bWx7v3u/jX1Fbo5CWWpRcWZ+nq2SoZ6BkkJqXnJ+SmZeuq1SaUmaroWSQnFJYl5KYk5+XqqtUmVqsZK9nU1KYkkisjZDoE49Y3NDSyU7m4Ki/ILUopLM1GIFfTsbfZBSOwBQSwECFAAUAAAACABIcBZX4vyw/mAAAABrAAAACwAAAAAAAAAAAAAAAAAAAAAAc3lzRGF0YS54bWxQSwUGAAAAAAEAAQA5AAAAiQAAAAAA</t>
   </si>
 </sst>
 </file>
@@ -255,31 +255,31 @@
         <v>13</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="0" t="s">
         <v>14</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12">
@@ -295,7 +295,7 @@
         <v>20</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14">
@@ -332,7 +332,7 @@
         <v>24</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>169422809867</v>
+        <v>171973069195</v>
       </c>
     </row>
     <row r="20">
@@ -422,7 +422,7 @@
         <v>45</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>